<commit_message>
Reporting dashboard and modification of the import method to add a bit of data
</commit_message>
<xml_diff>
--- a/DemoEditor/resources/DemoEditor-BooksCatalog.xlsx
+++ b/DemoEditor/resources/DemoEditor-BooksCatalog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/03637740bd6430a5/Edition/Packt - Clean Architecture .NET/Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Github\PacktPublishing\.NET-Architecture-for-Enterprise-Applications\DemoEditor\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="11_AD4D9D64A577C15A4A54185BD05D4EC05BDEDD93" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD159B58-452E-4518-902B-0CCD80FB7503}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4959A259-455A-4116-9969-75FFA77DF954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1425" yWindow="330" windowWidth="19860" windowHeight="19710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Books" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>ISBN</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>Not a rewrite, more of a completion of first edition</t>
+  </si>
+  <si>
+    <t>### FINISHED</t>
   </si>
 </sst>
 </file>
@@ -524,11 +527,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.85546875" bestFit="1" customWidth="1"/>
@@ -572,6 +573,9 @@
       <c r="C2" t="s">
         <v>14</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
       <c r="E2" t="s">
         <v>36</v>
       </c>
@@ -589,11 +593,17 @@
       <c r="C3" t="s">
         <v>16</v>
       </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
       <c r="E3" t="s">
         <v>37</v>
       </c>
       <c r="F3">
         <v>567</v>
+      </c>
+      <c r="G3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -606,6 +616,9 @@
       <c r="C4" t="s">
         <v>15</v>
       </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
       <c r="E4" t="s">
         <v>38</v>
       </c>
@@ -626,6 +639,9 @@
       <c r="C5" t="s">
         <v>17</v>
       </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
       <c r="E5" t="s">
         <v>39</v>
       </c>
@@ -666,6 +682,9 @@
       <c r="C7" t="s">
         <v>15</v>
       </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
       <c r="E7" t="s">
         <v>46</v>
       </c>
@@ -683,6 +702,9 @@
       <c r="C8" t="s">
         <v>19</v>
       </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
       <c r="E8" t="s">
         <v>48</v>
       </c>
@@ -703,6 +725,9 @@
       <c r="C9" t="s">
         <v>21</v>
       </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
       <c r="E9" t="s">
         <v>50</v>
       </c>
@@ -720,11 +745,17 @@
       <c r="C10" t="s">
         <v>20</v>
       </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
       <c r="E10" t="s">
         <v>49</v>
       </c>
       <c r="F10">
         <v>1034</v>
+      </c>
+      <c r="G10" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -736,6 +767,9 @@
       </c>
       <c r="C11" t="s">
         <v>15</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
       </c>
       <c r="E11" t="s">
         <v>47</v>

</xml_diff>